<commit_message>
feat(Permission): add seed permission
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/object_image.xlsx
+++ b/src/storage/app/excel-exporter/templates/object_image.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Camera</t>
   </si>
   <si>
+    <t xml:space="preserve">Hình ảnh</t>
+  </si>
+  <si>
     <t xml:space="preserve">[number]</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">[camera]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[image]</t>
   </si>
 </sst>
 </file>
@@ -150,10 +156,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,22 +187,28 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="92.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>